<commit_message>
Feedback, October 2023, code
And analysis of psychometric factors as a function of observation time
</commit_message>
<xml_diff>
--- a/data/battery_vars.xlsx
+++ b/data/battery_vars.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="358">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Age at the accident</t>
   </si>
   <si>
+    <t xml:space="preserve">age at the accident</t>
+  </si>
+  <si>
     <t xml:space="preserve">years</t>
   </si>
   <si>
@@ -76,10 +79,10 @@
     <t xml:space="preserve">age_interview</t>
   </si>
   <si>
-    <t xml:space="preserve">Age at the interview</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age, interview</t>
+    <t xml:space="preserve">Age at the survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age at the survey</t>
   </si>
   <si>
     <t xml:space="preserve">age_class</t>
@@ -91,7 +94,7 @@
     <t xml:space="preserve">Age class at the accident: young (up to 30), middle (31 – 65), elderly (66 and more years)</t>
   </si>
   <si>
-    <t xml:space="preserve">age class</t>
+    <t xml:space="preserve">age at the accident, class</t>
   </si>
   <si>
     <t xml:space="preserve">obs_time</t>
@@ -142,31 +145,34 @@
     <t xml:space="preserve">Highest education</t>
   </si>
   <si>
+    <t xml:space="preserve">highest education grade</t>
+  </si>
+  <si>
     <t xml:space="preserve">employment_status</t>
   </si>
   <si>
     <t xml:space="preserve">Employment status</t>
   </si>
   <si>
-    <t xml:space="preserve">employment</t>
+    <t xml:space="preserve">employment at the accident</t>
   </si>
   <si>
     <t xml:space="preserve">sport_profession</t>
   </si>
   <si>
-    <t xml:space="preserve">Sport-related profession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sport profession</t>
+    <t xml:space="preserve">Mountain sport-related profession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mountain sport profession</t>
   </si>
   <si>
     <t xml:space="preserve">trauma_risk_profession</t>
   </si>
   <si>
-    <t xml:space="preserve">Trauma-risk profession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trauma-risk profession</t>
+    <t xml:space="preserve">Search and rescue service profession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search and rescue profession</t>
   </si>
   <si>
     <t xml:space="preserve">medical_profession</t>
@@ -250,10 +256,10 @@
     <t xml:space="preserve">psych_comorbidity</t>
   </si>
   <si>
-    <t xml:space="preserve">Mental disorder prior to the accident</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pre-existing mental disorder</t>
+    <t xml:space="preserve">Professionally diagnosed mental disorder prior to the accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-existing diagnosed mental disorder</t>
   </si>
   <si>
     <t xml:space="preserve">traumatic_event</t>
@@ -298,10 +304,10 @@
     <t xml:space="preserve">prior_accident</t>
   </si>
   <si>
-    <t xml:space="preserve">Prior sport accidents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prior sport accidents</t>
+    <t xml:space="preserve">Prior mountain sport accidents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prior mountain sport accidents</t>
   </si>
   <si>
     <t xml:space="preserve">accident_year</t>
@@ -316,10 +322,10 @@
     <t xml:space="preserve">sport_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Type of sport at the accident</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sport type</t>
+    <t xml:space="preserve">Type of mountain sport at the accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mountain sport type</t>
   </si>
   <si>
     <t xml:space="preserve">accident_alone</t>
@@ -343,28 +349,28 @@
     <t xml:space="preserve">accident_injured_persons</t>
   </si>
   <si>
-    <t xml:space="preserve">Accident injured persons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">injured persons</t>
+    <t xml:space="preserve">Number of injured persons during the mountain sport accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of injured persons</t>
   </si>
   <si>
     <t xml:space="preserve">accident_rescue</t>
   </si>
   <si>
-    <t xml:space="preserve">Accident rescue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rescue</t>
+    <t xml:space="preserve">Mode of accident rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rescue mode</t>
   </si>
   <si>
     <t xml:space="preserve">accident_rescue_mode</t>
   </si>
   <si>
-    <t xml:space="preserve">Accident rescue mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rescue mode</t>
+    <t xml:space="preserve">Mode of professional accident rescue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">professional rescue mode</t>
   </si>
   <si>
     <t xml:space="preserve">injury_sev_strata</t>
@@ -493,10 +499,10 @@
     <t xml:space="preserve">surgery_done</t>
   </si>
   <si>
-    <t xml:space="preserve">Need for surgical therapy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">surgery</t>
+    <t xml:space="preserve">Surgical therapy of the accident’s injuries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surgical therapy</t>
   </si>
   <si>
     <t xml:space="preserve">surgery_complexity</t>
@@ -514,25 +520,25 @@
     <t xml:space="preserve">Psychological support or therapy after the accident</t>
   </si>
   <si>
-    <t xml:space="preserve">psychological support</t>
+    <t xml:space="preserve">psychological/psychiatric support post accident</t>
   </si>
   <si>
     <t xml:space="preserve">psych_support_need </t>
   </si>
   <si>
-    <t xml:space="preserve">Subjective need for psychological support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">psychological support need</t>
+    <t xml:space="preserve">Subjective need for psychological support after the accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psychological/psychiatric support need post accident</t>
   </si>
   <si>
     <t xml:space="preserve">accident_aftermath</t>
   </si>
   <si>
-    <t xml:space="preserve">Accident consequences felt, physical health health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">physical health consequences</t>
+    <t xml:space="preserve">Physical health consequences related to the accident </t>
+  </si>
+  <si>
+    <t xml:space="preserve">physical health consequences of the accident</t>
   </si>
   <si>
     <t xml:space="preserve">Alpine accident outcome</t>
@@ -544,46 +550,46 @@
     <t xml:space="preserve">same_sport_type_post_accident</t>
   </si>
   <si>
-    <t xml:space="preserve">Returned to the same sport activity post accident</t>
-  </si>
-  <si>
-    <t xml:space="preserve">returned to same sport</t>
+    <t xml:space="preserve">Returned to the same mountain sport activity following the accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">returned to same mountain sport post accident</t>
   </si>
   <si>
     <t xml:space="preserve">caution_post_accident</t>
   </si>
   <si>
-    <t xml:space="preserve">Caution after accident</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caution post accident</t>
+    <t xml:space="preserve">Caution during mountain sport activity after the accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caution during mountain sport post accident</t>
   </si>
   <si>
     <t xml:space="preserve">unwilling_flashback</t>
   </si>
   <si>
-    <t xml:space="preserve">Flashback during sport activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flashbacks during sport</t>
+    <t xml:space="preserve">Flashback during mountain sport activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flashbacks during mountain sport</t>
   </si>
   <si>
     <t xml:space="preserve">flashback_frequency</t>
   </si>
   <si>
-    <t xml:space="preserve">Flashback frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flashback frequency</t>
+    <t xml:space="preserve">Frequency of flashbacks during mountain sport activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flashback frequency during mountain sport</t>
   </si>
   <si>
     <t xml:space="preserve">confusion_during_sport</t>
   </si>
   <si>
-    <t xml:space="preserve">Confusion during sport activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confusion during sport</t>
+    <t xml:space="preserve">Confusion during mountain sport activity after the accident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confusion during mountain sport</t>
   </si>
   <si>
     <t xml:space="preserve">dsm5_total</t>
@@ -616,7 +622,7 @@
     <t xml:space="preserve">At least one PCL-5 domain positive</t>
   </si>
   <si>
-    <t xml:space="preserve">PTSD+ (at least one PCL-5 domain)</t>
+    <t xml:space="preserve">PTSD symptoms (at least one PCL-5 domain positive)</t>
   </si>
   <si>
     <t xml:space="preserve">main cutoff</t>
@@ -862,13 +868,13 @@
     <t xml:space="preserve">phq9_total_class</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9 score, depression symptoms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depression symptoms (PHQ-9 ≥11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depression symptoms, PHQ-9</t>
+    <t xml:space="preserve">PHQ-9 score ≥ 11 points, clinically relevant depressive symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinically relevant depression symptoms (PHQ-9 ≥11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinically relevant depression symptoms, PHQ-9</t>
   </si>
   <si>
     <t xml:space="preserve">gad7_total</t>
@@ -886,13 +892,13 @@
     <t xml:space="preserve">gad7_total_class</t>
   </si>
   <si>
-    <t xml:space="preserve">GAD-7 score, anxiety symptoms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anxiety symptoms (GAD-7 ≥10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anxiety symptoms, GAD-7</t>
+    <t xml:space="preserve">GAD-7 score ≥ 10 points, clinically relevant anxiety symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinically relevant anxiety symptoms (GAD-7 ≥10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinically relevant anxiety symptoms, GAD-7</t>
   </si>
   <si>
     <t xml:space="preserve">phqd_panic_total</t>
@@ -913,10 +919,10 @@
     <t xml:space="preserve">PHQ panic positivity</t>
   </si>
   <si>
-    <t xml:space="preserve">Panic symptoms (PHQ-panic)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panic symptoms, PHQ-panic</t>
+    <t xml:space="preserve">clinically relevant panic symptoms (PHQ-panic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinically relevant panic symptoms, PHQ-panic</t>
   </si>
   <si>
     <t xml:space="preserve">phq_events_total</t>
@@ -928,16 +934,19 @@
     <t xml:space="preserve">PHQ-15 score</t>
   </si>
   <si>
-    <t xml:space="preserve">Somatic symptoms, PHQ-15</t>
+    <t xml:space="preserve">Somatization symptoms, PHQ-15</t>
   </si>
   <si>
     <t xml:space="preserve">phq_events_total_class</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-15 health problems, clinically relevant somatic symptoms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Somatic symptoms (PHQ-15 ≥11)</t>
+    <t xml:space="preserve">PHQ-15 score ≥ 11 points, clinically relevant somatization symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinically relevant somatizaton symptoms (PHQ-15 ≥11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinically relevant somatization symptoms, PHQ-15</t>
   </si>
   <si>
     <t xml:space="preserve">eurohis_total</t>
@@ -1287,11 +1296,11 @@
   </sheetPr>
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.87"/>
@@ -1346,2605 +1355,2605 @@
         <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="26" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I58" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="J58" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J72" s="3"/>
     </row>
     <row r="73" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="75" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="79" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="80" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="83" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="84" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="85" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="86" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="E87" s="6"/>
       <c r="F87" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C88" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I88" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="J88" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D97" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="F97" s="1" t="s">
-        <v>339</v>
-      </c>
       <c r="G97" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>